<commit_message>
more gams and model  evaluation
</commit_message>
<xml_diff>
--- a/Model_evaluation.xlsx
+++ b/Model_evaluation.xlsx
@@ -16,43 +16,133 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>c5</t>
-  </si>
-  <si>
-    <t>c5.1</t>
-  </si>
-  <si>
-    <t>M_gam1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
     <t>Model</t>
   </si>
   <si>
-    <t>c5.2</t>
-  </si>
-  <si>
     <t>AIC_male</t>
   </si>
   <si>
     <t>AIC_female</t>
   </si>
   <si>
-    <t>Dev_male</t>
-  </si>
-  <si>
-    <t>Dev_female</t>
-  </si>
-  <si>
-    <t>c5.3</t>
+    <t>m1m2</t>
+  </si>
+  <si>
+    <t>s1s2</t>
+  </si>
+  <si>
+    <t>m1s1</t>
+  </si>
+  <si>
+    <t>m2s2</t>
+  </si>
+  <si>
+    <t>omitting snow winter and tautumn.mean</t>
+  </si>
+  <si>
+    <t>omitting  tsummer1.mean and r_newsummer1</t>
+  </si>
+  <si>
+    <t>omitting  tsummer1.mean and tautumn.mean</t>
+  </si>
+  <si>
+    <t>new colinearity check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">omitting snow_winter2 and  r_newsummer1 </t>
+  </si>
+  <si>
+    <t>M/F_x1.1</t>
+  </si>
+  <si>
+    <t>M/F_x1.2</t>
+  </si>
+  <si>
+    <t>M/F_x1.3</t>
+  </si>
+  <si>
+    <t>M/F_x1.4</t>
+  </si>
+  <si>
+    <t>replacement due to collinearity</t>
+  </si>
+  <si>
+    <t>PCA</t>
+  </si>
+  <si>
+    <t>NDVI summer1 and summer2</t>
+  </si>
+  <si>
+    <t>NDVI may1 and may2</t>
+  </si>
+  <si>
+    <t>M/F_x2.1</t>
+  </si>
+  <si>
+    <t>M/F_x2.2</t>
+  </si>
+  <si>
+    <t>M/F_x2.3</t>
+  </si>
+  <si>
+    <t>M/F_x2.4</t>
+  </si>
+  <si>
+    <t>M/F_x3.1</t>
+  </si>
+  <si>
+    <t>NDVI may1 and summer1</t>
+  </si>
+  <si>
+    <t>M/F_x3.2</t>
+  </si>
+  <si>
+    <t>M/F_x3.3</t>
+  </si>
+  <si>
+    <t>M/F_x3.4</t>
+  </si>
+  <si>
+    <t>M/F_x4.1</t>
+  </si>
+  <si>
+    <t>NDVI may2 and summer2</t>
+  </si>
+  <si>
+    <t>M/F_x4.2</t>
+  </si>
+  <si>
+    <t>M/F_x4.3</t>
+  </si>
+  <si>
+    <t>M/F_x4.4</t>
+  </si>
+  <si>
+    <t>M/Fq1</t>
+  </si>
+  <si>
+    <t>NVDI or replacement</t>
+  </si>
+  <si>
+    <t>Perc. area aperta</t>
+  </si>
+  <si>
+    <t>q_media</t>
+  </si>
+  <si>
+    <t>M/Faa1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> including snow winter and r_new summer1 has mostly best AIC in female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,16 +150,64 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -77,19 +215,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCC66"/>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,115 +632,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="105" zoomScaleNormal="105" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="15"/>
+    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="27">
+        <v>11950.88</v>
+      </c>
+      <c r="C3">
+        <v>9915.9840000000004</v>
+      </c>
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="28">
+        <v>11950.85</v>
+      </c>
+      <c r="C4">
+        <v>9915.6610000000001</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="27">
+        <v>11952.13</v>
+      </c>
+      <c r="C5">
+        <v>9917.68</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H5" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="29">
+        <v>11952.24</v>
+      </c>
+      <c r="C6" s="13">
+        <v>9912.5560000000005</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H6" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="16">
+        <v>11965.54</v>
+      </c>
+      <c r="C7">
+        <v>9918.7389999999996</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="16">
+        <v>11965.54</v>
+      </c>
+      <c r="C8">
+        <v>9918.5930000000008</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="20">
+        <v>11965.75</v>
+      </c>
+      <c r="C9">
+        <v>9916.4439999999995</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>11975.4</v>
-      </c>
-      <c r="C2">
-        <v>9922.8889999999992</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.33200000000000002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>11960.16</v>
-      </c>
-      <c r="C3">
-        <v>9911.1090000000004</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.32200000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>11960.16</v>
-      </c>
-      <c r="C4">
-        <v>9910.3960000000006</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.32300000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="10" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="21">
+        <v>11965.75</v>
+      </c>
+      <c r="C10" s="12">
+        <v>9916.4439999999995</v>
+      </c>
+      <c r="D10" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="E10" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15">
+        <v>11966.55</v>
+      </c>
+      <c r="C11">
+        <v>9919.0300000000007</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="15">
+        <v>11966.55</v>
+      </c>
+      <c r="C12">
+        <v>9919.0300000000007</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="16">
+        <v>11965.3</v>
+      </c>
+      <c r="C13" s="10">
+        <v>9916.2939999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="17">
+        <v>11965.3</v>
+      </c>
+      <c r="C14" s="11">
+        <v>9916.348</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="15">
+        <v>11963.36</v>
+      </c>
+      <c r="C15">
+        <v>9918.6329999999998</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="16">
+        <v>11962.41</v>
+      </c>
+      <c r="C16">
+        <v>9918.7579999999998</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="15">
+        <v>11963.18</v>
+      </c>
+      <c r="C17" s="10">
+        <v>9917.6229999999996</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="25" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="25">
+        <v>11963.18</v>
+      </c>
+      <c r="C18" s="26">
+        <v>9917.6229999999996</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="22">
+        <v>11966.58</v>
+      </c>
+      <c r="C19" s="23">
+        <v>9913.4390000000003</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E19" s="18"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="15">
         <v>11965.76</v>
       </c>
-      <c r="C5">
-        <v>9918.3080000000009</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0.318</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>9908.0920000000006</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0.38300000000000001</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.32100000000000001</v>
-      </c>
+      <c r="C20" s="24">
+        <v>9916.232</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>